<commit_message>
Added data driven testcases using DataDriver library
</commit_message>
<xml_diff>
--- a/Data/Test_Data/Data.xlsx
+++ b/Data/Test_Data/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="854"/>
   </bookViews>
   <sheets>
     <sheet name="Invalid_Login_Credentials" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>${username}</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Jane</t>
   </si>
 </sst>
 </file>
@@ -69,8 +75,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,15 +363,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="30.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -367,12 +382,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -380,12 +398,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R8" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>